<commit_message>
MD5 blog, almost done
</commit_message>
<xml_diff>
--- a/aoc/d2runtimes.xlsx
+++ b/aoc/d2runtimes.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12660" activeTab="1"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -79,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -128,7 +128,7 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -152,40 +152,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="9">
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -292,6 +262,24 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -308,7 +296,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Sachin V. Shah" refreshedDate="42834.611951157407" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="25">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="42834.611951157407" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="25">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F26" sheet="Sheet1"/>
   </cacheSource>
@@ -578,7 +566,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -683,10 +671,10 @@
     <dataField name="Average of Gen2" fld="5" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="11">
+    <format dxfId="8">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -710,13 +698,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A19:F24" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A19:F24" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" dataCellStyle="Percent">
   <tableColumns count="6">
     <tableColumn id="1" name="Algorithm"/>
-    <tableColumn id="2" name="Real" dataDxfId="10" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="CPU" dataDxfId="9" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Gen0" dataDxfId="8" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Gen1" dataDxfId="7" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="Real" dataDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="CPU" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Gen0" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Gen1" dataDxfId="1" dataCellStyle="Percent"/>
     <tableColumn id="6" name="Gen2" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1848,8 +1836,9 @@
     <sortCondition ref="B20:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>